<commit_message>
Added new variable and data visualizations, lin reg chunks
</commit_message>
<xml_diff>
--- a/data/raw/r_household_survey_analysis.xlsx
+++ b/data/raw/r_household_survey_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Accra and Fulbright/Data/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{0396615F-A6F1-C64B-97F4-342526E7FE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B129343-42D9-2C49-8DF4-FB186634C704}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{0396615F-A6F1-C64B-97F4-342526E7FE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{583EB046-4D2B-E642-AC6E-68AA37DE18AA}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{3AF34A9D-8751-B74B-BB26-3005C40DF547}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3AF34A9D-8751-B74B-BB26-3005C40DF547}"/>
   </bookViews>
   <sheets>
     <sheet name="important pieces" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,6 @@
     <t>tailoring</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>delivered</t>
   </si>
   <si>
@@ -552,6 +549,9 @@
   </si>
   <si>
     <t>hhhead_relation</t>
+  </si>
+  <si>
+    <t>piped_point_dist_km</t>
   </si>
 </sst>
 </file>
@@ -613,6 +613,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -912,9 +916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ED95C1-6467-C043-B50B-C26DEC2BEE04}">
-  <dimension ref="A1:AA117"/>
+  <dimension ref="A1:AB117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -930,9 +936,10 @@
     <col min="22" max="23" width="10.83203125" style="1"/>
     <col min="26" max="26" width="46.1640625" customWidth="1"/>
     <col min="27" max="27" width="19.83203125" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -961,7 +968,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1014,8 +1021,11 @@
       <c r="AA1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1056,7 +1066,7 @@
         <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -1092,13 +1102,16 @@
         <v>2</v>
       </c>
       <c r="Z2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB2">
+        <v>4.0753236086553596E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1175,13 +1188,16 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AA3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB3">
+        <v>2.8342272858933957E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1222,7 +1238,7 @@
         <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O4" t="s">
         <v>46</v>
@@ -1258,13 +1274,16 @@
         <v>2</v>
       </c>
       <c r="Z4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB4">
+        <v>2.4288161965156419E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1305,7 +1324,7 @@
         <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -1346,8 +1365,11 @@
       <c r="AA5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB5">
+        <v>8.9405550404061084E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1388,7 +1410,7 @@
         <v>32</v>
       </c>
       <c r="N6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O6" t="s">
         <v>34</v>
@@ -1424,13 +1446,16 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB6">
+        <v>2.0167372860979336E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1507,13 +1532,16 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB7">
+        <v>4.3125650423060907E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1554,7 +1582,7 @@
         <v>32</v>
       </c>
       <c r="N8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O8" t="s">
         <v>31</v>
@@ -1590,13 +1618,16 @@
         <v>2</v>
       </c>
       <c r="Z8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB8">
+        <v>2.9630027759640434E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1673,13 +1704,16 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB9">
+        <v>1.2264736875373492E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1720,7 +1754,7 @@
         <v>32</v>
       </c>
       <c r="N10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O10" t="s">
         <v>31</v>
@@ -1756,13 +1790,16 @@
         <v>2</v>
       </c>
       <c r="Z10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB10">
+        <v>1.0177599181934966E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1839,13 +1876,16 @@
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB11">
+        <v>1.7317520120156464E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1927,8 +1967,11 @@
       <c r="AA12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB12">
+        <v>6.7471620869153145E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1969,7 +2012,7 @@
         <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O13" t="s">
         <v>32</v>
@@ -2005,13 +2048,16 @@
         <v>1</v>
       </c>
       <c r="Z13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AA13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB13">
+        <v>1.623175966955168E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2088,13 +2134,16 @@
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB14">
+        <v>1.002779523795135E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2171,13 +2220,16 @@
         <v>0</v>
       </c>
       <c r="Z15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB15">
+        <v>2.4631675178540348E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2254,13 +2306,16 @@
         <v>2</v>
       </c>
       <c r="Z16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB16">
+        <v>1.2237056893657934E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2301,7 +2356,7 @@
         <v>32</v>
       </c>
       <c r="N17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O17" t="s">
         <v>31</v>
@@ -2342,8 +2397,11 @@
       <c r="AA17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB17">
+        <v>0.10713850783604233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2420,13 +2478,16 @@
         <v>0</v>
       </c>
       <c r="Z18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB18">
+        <v>0.12096147685383697</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2508,8 +2569,11 @@
       <c r="AA19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB19">
+        <v>0.18011176859191552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2550,7 +2614,7 @@
         <v>32</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O20" t="s">
         <v>31</v>
@@ -2586,13 +2650,16 @@
         <v>0</v>
       </c>
       <c r="Z20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB20">
+        <v>0.14499697231191069</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2633,7 +2700,7 @@
         <v>32</v>
       </c>
       <c r="N21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O21" t="s">
         <v>31</v>
@@ -2674,8 +2741,11 @@
       <c r="AA21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB21">
+        <v>0.14615593544604188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2757,8 +2827,11 @@
       <c r="AA22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB22">
+        <v>0.15400599577703983</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2840,8 +2913,11 @@
       <c r="AA23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB23">
+        <v>0.11946849012437082</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2882,13 +2958,13 @@
         <v>32</v>
       </c>
       <c r="N24" t="s">
+        <v>126</v>
+      </c>
+      <c r="O24" t="s">
+        <v>34</v>
+      </c>
+      <c r="P24" t="s">
         <v>127</v>
-      </c>
-      <c r="O24" t="s">
-        <v>34</v>
-      </c>
-      <c r="P24" t="s">
-        <v>128</v>
       </c>
       <c r="Q24" t="s">
         <v>33</v>
@@ -2923,8 +2999,11 @@
       <c r="AA24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB24">
+        <v>6.5630509500441164E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2965,7 +3044,7 @@
         <v>32</v>
       </c>
       <c r="N25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O25" t="s">
         <v>31</v>
@@ -3006,8 +3085,11 @@
       <c r="AA25" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB25">
+        <v>2.6127603615269491E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3048,7 +3130,7 @@
         <v>32</v>
       </c>
       <c r="N26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O26" t="s">
         <v>34</v>
@@ -3084,13 +3166,16 @@
         <v>0</v>
       </c>
       <c r="Z26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB26">
+        <v>5.4088798751585086E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3131,7 +3216,7 @@
         <v>32</v>
       </c>
       <c r="N27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O27" t="s">
         <v>31</v>
@@ -3167,13 +3252,16 @@
         <v>4</v>
       </c>
       <c r="Z27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA27" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB27">
+        <v>9.8678704003806491E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3250,13 +3338,16 @@
         <v>0.5</v>
       </c>
       <c r="Z28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB28">
+        <v>3.5100188858478919E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3303,7 +3394,7 @@
         <v>34</v>
       </c>
       <c r="P29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q29" t="s">
         <v>48</v>
@@ -3338,8 +3429,11 @@
       <c r="AA29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB29">
+        <v>5.2306402880864661E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3380,7 +3474,7 @@
         <v>32</v>
       </c>
       <c r="N30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O30" t="s">
         <v>31</v>
@@ -3416,13 +3510,16 @@
         <v>1</v>
       </c>
       <c r="Z30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB30">
+        <v>4.9614484749507248E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3463,7 +3560,7 @@
         <v>34</v>
       </c>
       <c r="N31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O31" t="s">
         <v>32</v>
@@ -3499,13 +3596,16 @@
         <v>0</v>
       </c>
       <c r="Z31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB31">
+        <v>7.6971996779444482E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3582,13 +3682,16 @@
         <v>0</v>
       </c>
       <c r="Z32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB32">
+        <v>2.2580216135793977E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3629,13 +3732,13 @@
         <v>32</v>
       </c>
       <c r="N33" t="s">
+        <v>134</v>
+      </c>
+      <c r="O33" t="s">
+        <v>32</v>
+      </c>
+      <c r="P33" t="s">
         <v>135</v>
-      </c>
-      <c r="O33" t="s">
-        <v>32</v>
-      </c>
-      <c r="P33" t="s">
-        <v>136</v>
       </c>
       <c r="Q33" t="s">
         <v>33</v>
@@ -3665,13 +3768,16 @@
         <v>0</v>
       </c>
       <c r="Z33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB33">
+        <v>5.1286771120905149E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3712,7 +3818,7 @@
         <v>32</v>
       </c>
       <c r="N34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O34" t="s">
         <v>31</v>
@@ -3748,13 +3854,16 @@
         <v>2</v>
       </c>
       <c r="Z34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA34" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB34">
+        <v>3.4343816392174945E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3795,7 +3904,7 @@
         <v>32</v>
       </c>
       <c r="N35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O35" t="s">
         <v>31</v>
@@ -3836,8 +3945,11 @@
       <c r="AA35" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB35">
+        <v>1.6985595576662717E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3878,7 +3990,7 @@
         <v>32</v>
       </c>
       <c r="N36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O36" t="s">
         <v>31</v>
@@ -3919,8 +4031,11 @@
       <c r="AA36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB36">
+        <v>6.6499364631437852E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3961,7 +4076,7 @@
         <v>32</v>
       </c>
       <c r="N37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O37" t="s">
         <v>31</v>
@@ -3997,13 +4112,16 @@
         <v>0</v>
       </c>
       <c r="Z37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA37" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB37">
+        <v>9.5941596290054942E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4044,7 +4162,7 @@
         <v>32</v>
       </c>
       <c r="N38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O38" t="s">
         <v>31</v>
@@ -4080,13 +4198,16 @@
         <v>0</v>
       </c>
       <c r="Z38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA38" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB38">
+        <v>7.8055853310960835E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4133,7 +4254,7 @@
         <v>32</v>
       </c>
       <c r="P39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q39" t="s">
         <v>33</v>
@@ -4168,8 +4289,11 @@
       <c r="AA39" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB39">
+        <v>0.16670064462429279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4210,7 +4334,7 @@
         <v>32</v>
       </c>
       <c r="N40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O40" t="s">
         <v>31</v>
@@ -4246,13 +4370,16 @@
         <v>0</v>
       </c>
       <c r="Z40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA40" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB40">
+        <v>6.235747115182786E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4293,7 +4420,7 @@
         <v>32</v>
       </c>
       <c r="N41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O41" t="s">
         <v>31</v>
@@ -4329,13 +4456,16 @@
         <v>0</v>
       </c>
       <c r="Z41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB41">
+        <v>9.0662126266865276E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4376,7 +4506,7 @@
         <v>32</v>
       </c>
       <c r="N42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O42" t="s">
         <v>31</v>
@@ -4412,13 +4542,16 @@
         <v>0</v>
       </c>
       <c r="Z42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA42" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB42">
+        <v>3.8223569663314798E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4459,7 +4592,7 @@
         <v>32</v>
       </c>
       <c r="N43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O43" t="s">
         <v>31</v>
@@ -4500,8 +4633,11 @@
       <c r="AA43" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB43">
+        <v>5.1782921810136967E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4542,7 +4678,7 @@
         <v>32</v>
       </c>
       <c r="N44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O44" t="s">
         <v>31</v>
@@ -4583,8 +4719,11 @@
       <c r="AA44" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB44">
+        <v>1.7737108006762748E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4625,7 +4764,7 @@
         <v>32</v>
       </c>
       <c r="N45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O45" t="s">
         <v>31</v>
@@ -4666,8 +4805,11 @@
       <c r="AA45" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB45">
+        <v>0.12188327954647341</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4726,7 +4868,7 @@
         <v>76</v>
       </c>
       <c r="T46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U46" t="s">
         <v>49</v>
@@ -4744,13 +4886,16 @@
         <v>0</v>
       </c>
       <c r="Z46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA46" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB46">
+        <v>7.304252051092E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4791,7 +4936,7 @@
         <v>32</v>
       </c>
       <c r="N47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O47" t="s">
         <v>31</v>
@@ -4832,8 +4977,11 @@
       <c r="AA47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB47">
+        <v>3.1146776355970757E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4874,7 +5022,7 @@
         <v>32</v>
       </c>
       <c r="N48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O48" t="s">
         <v>46</v>
@@ -4915,8 +5063,11 @@
       <c r="AA48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB48">
+        <v>1.455340913252102E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4957,7 +5108,7 @@
         <v>71</v>
       </c>
       <c r="N49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O49" t="s">
         <v>32</v>
@@ -4998,8 +5149,11 @@
       <c r="AA49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB49">
+        <v>2.8106752116164008E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5040,7 +5194,7 @@
         <v>32</v>
       </c>
       <c r="N50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O50" t="s">
         <v>31</v>
@@ -5081,8 +5235,11 @@
       <c r="AA50" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB50">
+        <v>1.7843102196074115E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5123,7 +5280,7 @@
         <v>32</v>
       </c>
       <c r="N51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O51" t="s">
         <v>32</v>
@@ -5159,13 +5316,16 @@
         <v>0</v>
       </c>
       <c r="Z51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA51" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB51">
+        <v>2.0324079462973096E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5206,7 +5366,7 @@
         <v>32</v>
       </c>
       <c r="N52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O52" t="s">
         <v>31</v>
@@ -5242,13 +5402,16 @@
         <v>0</v>
       </c>
       <c r="Z52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AA52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB52">
+        <v>1.9391831029314917E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5289,7 +5452,7 @@
         <v>32</v>
       </c>
       <c r="N53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O53" t="s">
         <v>31</v>
@@ -5325,13 +5488,16 @@
         <v>1</v>
       </c>
       <c r="Z53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA53" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB53">
+        <v>3.792721962634852E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5408,13 +5574,16 @@
         <v>0</v>
       </c>
       <c r="Z54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB54">
+        <v>7.9334922246218492E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5455,7 +5624,7 @@
         <v>32</v>
       </c>
       <c r="N55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O55" t="s">
         <v>34</v>
@@ -5491,13 +5660,16 @@
         <v>1</v>
       </c>
       <c r="Z55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AA55" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB55">
+        <v>5.163949026942671E-6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5538,7 +5710,7 @@
         <v>71</v>
       </c>
       <c r="N56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O56" t="s">
         <v>32</v>
@@ -5579,8 +5751,11 @@
       <c r="AA56" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB56">
+        <v>1.9740361770163899E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5657,13 +5832,16 @@
         <v>1</v>
       </c>
       <c r="Z57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AA57" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB57">
+        <v>3.1330982605283858E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5745,8 +5923,11 @@
       <c r="AA58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB58">
+        <v>5.1859882496751233E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5823,13 +6004,16 @@
         <v>2.5</v>
       </c>
       <c r="Z59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA59" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB59">
+        <v>1.22038124099462E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5870,7 +6054,7 @@
         <v>32</v>
       </c>
       <c r="N60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O60" t="s">
         <v>31</v>
@@ -5911,8 +6095,11 @@
       <c r="AA60" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB60">
+        <v>1.3660915739534155E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5994,8 +6181,11 @@
       <c r="AA61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB61">
+        <v>2.9925530946143961E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6077,8 +6267,11 @@
       <c r="AA62" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB62">
+        <v>2.9833207512362434E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6155,13 +6348,16 @@
         <v>0</v>
       </c>
       <c r="Z63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA63" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB63">
+        <v>3.0661853322792237E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6238,13 +6434,16 @@
         <v>3</v>
       </c>
       <c r="Z64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA64" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB64">
+        <v>2.575505389414633E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6285,7 +6484,7 @@
         <v>32</v>
       </c>
       <c r="N65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O65" t="s">
         <v>31</v>
@@ -6326,8 +6525,11 @@
       <c r="AA65" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB65">
+        <v>2.3998849018698146E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6397,20 +6599,23 @@
       <c r="W66" s="1">
         <v>4.1224489795918364</v>
       </c>
-      <c r="X66" t="s">
-        <v>81</v>
+      <c r="X66">
+        <v>0</v>
       </c>
       <c r="Y66" s="2">
         <v>1</v>
       </c>
       <c r="Z66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA66" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB66">
+        <v>3.0780732251489799E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6451,7 +6656,7 @@
         <v>32</v>
       </c>
       <c r="N67" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O67" t="s">
         <v>31</v>
@@ -6487,13 +6692,16 @@
         <v>0</v>
       </c>
       <c r="Z67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AA67" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB67">
+        <v>1.8166670328200525E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6575,8 +6783,11 @@
       <c r="AA68" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB68">
+        <v>1.1776646148020134E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6617,7 +6828,7 @@
         <v>32</v>
       </c>
       <c r="N69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O69" t="s">
         <v>31</v>
@@ -6658,8 +6869,11 @@
       <c r="AA69" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB69">
+        <v>2.1435554837619868E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6741,8 +6955,11 @@
       <c r="AA70" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB70">
+        <v>1.5019427945066654E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6783,7 +7000,7 @@
         <v>32</v>
       </c>
       <c r="N71" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O71" t="s">
         <v>71</v>
@@ -6801,7 +7018,7 @@
         <v>71</v>
       </c>
       <c r="T71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U71" t="s">
         <v>35</v>
@@ -6824,8 +7041,11 @@
       <c r="AA71" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB71">
+        <v>1.0169824042645414E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6907,8 +7127,11 @@
       <c r="AA72" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB72">
+        <v>1.6223711992405691E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6949,7 +7172,7 @@
         <v>32</v>
       </c>
       <c r="N73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O73" t="s">
         <v>31</v>
@@ -6985,13 +7208,16 @@
         <v>3.5</v>
       </c>
       <c r="Z73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA73" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB73">
+        <v>2.2788918506284967E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -7032,7 +7258,7 @@
         <v>32</v>
       </c>
       <c r="N74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O74" t="s">
         <v>34</v>
@@ -7073,8 +7299,11 @@
       <c r="AA74" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB74">
+        <v>4.6010910737512879E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -7133,7 +7362,7 @@
         <v>34</v>
       </c>
       <c r="T75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U75" t="s">
         <v>35</v>
@@ -7151,13 +7380,16 @@
         <v>3</v>
       </c>
       <c r="Z75" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA75" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB75">
+        <v>3.3127021805335395E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7234,13 +7466,16 @@
         <v>0</v>
       </c>
       <c r="Z76" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA76" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB76">
+        <v>2.8861823098049664E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7281,7 +7516,7 @@
         <v>32</v>
       </c>
       <c r="N77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O77" t="s">
         <v>31</v>
@@ -7322,8 +7557,11 @@
       <c r="AA77" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB77">
+        <v>4.1361016483721744E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7364,7 +7602,7 @@
         <v>32</v>
       </c>
       <c r="N78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O78" t="s">
         <v>31</v>
@@ -7405,8 +7643,11 @@
       <c r="AA78" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB78">
+        <v>3.028385588736586E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7488,8 +7729,11 @@
       <c r="AA79" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB79">
+        <v>3.3935694534280171E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7530,7 +7774,7 @@
         <v>32</v>
       </c>
       <c r="N80" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O80" t="s">
         <v>31</v>
@@ -7566,13 +7810,16 @@
         <v>0</v>
       </c>
       <c r="Z80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA80" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB80">
+        <v>1.8568015004405858E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7613,7 +7860,7 @@
         <v>32</v>
       </c>
       <c r="N81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O81" t="s">
         <v>31</v>
@@ -7654,8 +7901,11 @@
       <c r="AA81" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB81">
+        <v>1.3020988708426795E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7696,13 +7946,13 @@
         <v>32</v>
       </c>
       <c r="N82" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O82" t="s">
         <v>34</v>
       </c>
       <c r="P82" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q82" s="2" t="s">
         <v>48</v>
@@ -7714,7 +7964,7 @@
         <v>34</v>
       </c>
       <c r="T82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U82" t="s">
         <v>35</v>
@@ -7732,13 +7982,16 @@
         <v>4</v>
       </c>
       <c r="Z82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA82" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB82">
+        <v>1.9337811203272187E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7779,7 +8032,7 @@
         <v>32</v>
       </c>
       <c r="N83" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O83" t="s">
         <v>31</v>
@@ -7815,13 +8068,16 @@
         <v>0</v>
       </c>
       <c r="Z83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA83" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB83">
+        <v>2.5339552357798448E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7862,7 +8118,7 @@
         <v>32</v>
       </c>
       <c r="N84" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O84" t="s">
         <v>71</v>
@@ -7898,13 +8154,16 @@
         <v>2</v>
       </c>
       <c r="Z84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AA84" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB84">
+        <v>2.3004761305963243E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7981,13 +8240,16 @@
         <v>2</v>
       </c>
       <c r="Z85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA85" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB85">
+        <v>1.7605278974571165E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -8028,7 +8290,7 @@
         <v>32</v>
       </c>
       <c r="N86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O86" t="s">
         <v>31</v>
@@ -8064,13 +8326,16 @@
         <v>2</v>
       </c>
       <c r="Z86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AA86" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB86">
+        <v>2.4123860020810742E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -8111,7 +8376,7 @@
         <v>32</v>
       </c>
       <c r="N87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O87" t="s">
         <v>31</v>
@@ -8147,13 +8412,16 @@
         <v>0</v>
       </c>
       <c r="Z87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA87" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB87">
+        <v>1.7539748700446913E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8200,7 +8468,7 @@
         <v>34</v>
       </c>
       <c r="P88" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q88" t="s">
         <v>48</v>
@@ -8230,13 +8498,16 @@
         <v>0</v>
       </c>
       <c r="Z88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA88" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB88">
+        <v>9.0674614541575854E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8318,8 +8589,11 @@
       <c r="AA89" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB89">
+        <v>0.19479978968829048</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8360,7 +8634,7 @@
         <v>32</v>
       </c>
       <c r="N90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O90" t="s">
         <v>32</v>
@@ -8401,8 +8675,11 @@
       <c r="AA90" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB90">
+        <v>0.16470884529356233</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8443,7 +8720,7 @@
         <v>32</v>
       </c>
       <c r="N91" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O91" t="s">
         <v>34</v>
@@ -8461,7 +8738,7 @@
         <v>34</v>
       </c>
       <c r="T91" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U91" t="s">
         <v>35</v>
@@ -8479,13 +8756,16 @@
         <v>0</v>
       </c>
       <c r="Z91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA91" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB91">
+        <v>8.9024379993534519E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8526,7 +8806,7 @@
         <v>32</v>
       </c>
       <c r="N92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O92" t="s">
         <v>31</v>
@@ -8567,8 +8847,11 @@
       <c r="AA92" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB92">
+        <v>0.13113043041084863</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8609,7 +8892,7 @@
         <v>32</v>
       </c>
       <c r="N93" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O93" t="s">
         <v>31</v>
@@ -8650,8 +8933,11 @@
       <c r="AA93" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB93">
+        <v>0.12855839333833188</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8692,7 +8978,7 @@
         <v>32</v>
       </c>
       <c r="N94" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O94" t="s">
         <v>71</v>
@@ -8733,8 +9019,11 @@
       <c r="AA94" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB94">
+        <v>8.0481609295242409E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8775,7 +9064,7 @@
         <v>32</v>
       </c>
       <c r="N95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O95" t="s">
         <v>71</v>
@@ -8811,13 +9100,16 @@
         <v>0</v>
       </c>
       <c r="Z95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA95" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB95">
+        <v>0.16069392002074234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8861,10 +9153,10 @@
         <v>52</v>
       </c>
       <c r="O96" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q96" t="s">
         <v>33</v>
@@ -8894,13 +9186,16 @@
         <v>0</v>
       </c>
       <c r="Z96" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AA96" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB96">
+        <v>0.11658683811911161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8941,7 +9236,7 @@
         <v>32</v>
       </c>
       <c r="N97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O97" t="s">
         <v>31</v>
@@ -8982,8 +9277,11 @@
       <c r="AA97" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB97">
+        <v>3.8562986629979375E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -9065,8 +9363,11 @@
       <c r="AA98" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB98">
+        <v>0.1114519100236635</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -9107,7 +9408,7 @@
         <v>32</v>
       </c>
       <c r="N99" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O99" t="s">
         <v>32</v>
@@ -9148,8 +9449,11 @@
       <c r="AA99" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB99">
+        <v>5.2841042666974564E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9190,7 +9494,7 @@
         <v>32</v>
       </c>
       <c r="N100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O100" t="s">
         <v>31</v>
@@ -9226,13 +9530,16 @@
         <v>0</v>
       </c>
       <c r="Z100" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AA100" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB100">
+        <v>0.13214908129616573</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9273,7 +9580,7 @@
         <v>71</v>
       </c>
       <c r="N101" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O101" t="s">
         <v>31</v>
@@ -9314,8 +9621,11 @@
       <c r="AA101" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB101">
+        <v>0.16740808894481082</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9356,7 +9666,7 @@
         <v>71</v>
       </c>
       <c r="N102" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O102" t="s">
         <v>32</v>
@@ -9397,8 +9707,11 @@
       <c r="AA102" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB102">
+        <v>0.15410520174337169</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9480,8 +9793,11 @@
       <c r="AA103" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB103">
+        <v>0.13560064052214044</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9522,7 +9838,7 @@
         <v>32</v>
       </c>
       <c r="N104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O104" t="s">
         <v>31</v>
@@ -9558,13 +9874,16 @@
         <v>1</v>
       </c>
       <c r="Z104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA104" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB104">
+        <v>4.563265185162596E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -9641,13 +9960,16 @@
         <v>3</v>
       </c>
       <c r="Z105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AA105" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB105">
+        <v>8.9576393951429911E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -9688,13 +10010,13 @@
         <v>71</v>
       </c>
       <c r="N106" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O106" t="s">
         <v>32</v>
       </c>
       <c r="P106" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q106" t="s">
         <v>48</v>
@@ -9724,13 +10046,16 @@
         <v>0</v>
       </c>
       <c r="Z106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA106" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB106">
+        <v>9.2249075385733931E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -9771,7 +10096,7 @@
         <v>32</v>
       </c>
       <c r="N107" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O107" t="s">
         <v>34</v>
@@ -9807,13 +10132,16 @@
         <v>3</v>
       </c>
       <c r="Z107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AA107" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB107">
+        <v>7.2698776878339338E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9854,13 +10182,13 @@
         <v>32</v>
       </c>
       <c r="N108" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O108" t="s">
         <v>34</v>
       </c>
       <c r="P108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q108" t="s">
         <v>48</v>
@@ -9895,8 +10223,11 @@
       <c r="AA108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB108">
+        <v>0.11528740124474283</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9937,7 +10268,7 @@
         <v>32</v>
       </c>
       <c r="N109" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O109" t="s">
         <v>31</v>
@@ -9973,13 +10304,16 @@
         <v>0</v>
       </c>
       <c r="Z109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AA109" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB109">
+        <v>7.0986960212871819E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -10057,13 +10391,16 @@
         <v>3</v>
       </c>
       <c r="Z110" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA110" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB110">
+        <v>0.1718540028019106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -10104,7 +10441,7 @@
         <v>32</v>
       </c>
       <c r="N111" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O111" t="s">
         <v>71</v>
@@ -10145,8 +10482,11 @@
       <c r="AA111" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB111">
+        <v>4.6032588964989372E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -10223,13 +10563,16 @@
         <v>0</v>
       </c>
       <c r="Z112" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA112" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB112">
+        <v>8.972774630098404E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -10288,7 +10631,7 @@
         <v>34</v>
       </c>
       <c r="T113" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U113" t="s">
         <v>35</v>
@@ -10311,8 +10654,11 @@
       <c r="AA113" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB113">
+        <v>0.11479979743394296</v>
+      </c>
+    </row>
+    <row r="114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -10353,7 +10699,7 @@
         <v>32</v>
       </c>
       <c r="N114" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O114" t="s">
         <v>31</v>
@@ -10394,8 +10740,11 @@
       <c r="AA114" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB114">
+        <v>0.10469680508733631</v>
+      </c>
+    </row>
+    <row r="115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -10436,13 +10785,13 @@
         <v>32</v>
       </c>
       <c r="N115" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O115" t="s">
         <v>71</v>
       </c>
       <c r="P115" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q115" t="s">
         <v>48</v>
@@ -10477,8 +10826,11 @@
       <c r="AA115" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB115">
+        <v>0.15470477530183885</v>
+      </c>
+    </row>
+    <row r="116" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -10519,7 +10871,7 @@
         <v>32</v>
       </c>
       <c r="N116" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O116" t="s">
         <v>31</v>
@@ -10560,8 +10912,11 @@
       <c r="AA116" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB116">
+        <v>0.11679788069131729</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -10620,7 +10975,7 @@
         <v>71</v>
       </c>
       <c r="T117" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U117" t="s">
         <v>35</v>
@@ -10638,10 +10993,13 @@
         <v>0</v>
       </c>
       <c r="Z117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA117" t="s">
         <v>41</v>
+      </c>
+      <c r="AB117">
+        <v>0.1428220719481284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>